<commit_message>
Updated logging and invalidName test method Added
</commit_message>
<xml_diff>
--- a/testData/DataToValidateNameField.xlsx
+++ b/testData/DataToValidateNameField.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2457173_cognizant_com/Documents/Desktop/Training/Project Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2457173\IdeaProjects\PentagonProfileStats\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048C3F19C72185BDE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F274382-C795-4AAA-B8D8-2EAF601B816C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8E0C91-A151-4974-AB0A-F2D8DDD7DD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,52 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Sai</t>
-  </si>
-  <si>
-    <t>Konduru Bharath Sai</t>
-  </si>
-  <si>
-    <t>pavan789823</t>
-  </si>
-  <si>
-    <t>భారత</t>
-  </si>
-  <si>
-    <t>சாய்</t>
-  </si>
-  <si>
-    <t>Dhruv~!?_</t>
-  </si>
-  <si>
-    <t>पसन्द</t>
-  </si>
-  <si>
-    <t>Maheshhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>!@#$%^&amp;*()!@#$%^&amp;*()!@#$%^&amp;*()!@#$%^&amp;*(!@*(!@#$%^&amp;{:&gt;}!@#$%^&amp;*()!@#$%^&amp;*(@#$%^&amp;*(@#$%^&amp;*@#$%^&amp;*@#$%^&amp;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Bharath</t>
+  </si>
+  <si>
+    <t>Pavan</t>
+  </si>
+  <si>
+    <t>Dhruv</t>
+  </si>
+  <si>
+    <t>Santosh</t>
+  </si>
+  <si>
+    <t>Naveen</t>
+  </si>
+  <si>
+    <t>Kondurur Bharath Sai</t>
+  </si>
+  <si>
+    <t>KBS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8.3000000000000007"/>
-      <color rgb="FF6AAB73"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,14 +81,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,65 +363,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="159.5">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <v>1.2345678901234501E+115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="57.5">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>